<commit_message>
Adjust elec/CoESC to account for future projected inflation
</commit_message>
<xml_diff>
--- a/InputData/elec/CoESC/Cost of Electricity Sector Capital.xlsx
+++ b/InputData/elec/CoESC/Cost of Electricity Sector Capital.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\CoESC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE6014C-E3E5-4297-A412-B80CBDB6B0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683F7C9D-D7E7-4F9E-A227-E4444848B0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="1740" windowWidth="19680" windowHeight="21540" xr2:uid="{C8F9D547-902B-4E49-8BA2-E23B0A2DC1A9}"/>
+    <workbookView xWindow="5370" yWindow="3510" windowWidth="23970" windowHeight="18915" xr2:uid="{C8F9D547-902B-4E49-8BA2-E23B0A2DC1A9}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Lazard Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="CoESC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>CoESC Cost of Electricity Sector Capital</t>
   </si>
@@ -97,15 +97,69 @@
   </si>
   <si>
     <t>Unit: dimensionless (% of project cost)</t>
+  </si>
+  <si>
+    <t>Since the EPS works in real (inflation-adjusted) currency units, and interest rates are set by</t>
+  </si>
+  <si>
+    <t>banks and financial firms in nominal terms (factoring in their expectations of future inflation),</t>
+  </si>
+  <si>
+    <t>we need to adjust published interest rates by subtracting out the share that represents</t>
+  </si>
+  <si>
+    <t>inflation (i.e., the payment they demand just to keep up with inflation).</t>
+  </si>
+  <si>
+    <t>Inflation Adjustment</t>
+  </si>
+  <si>
+    <t>Data from Lazard</t>
+  </si>
+  <si>
+    <t>Future Inflation Estimate</t>
+  </si>
+  <si>
+    <t>U.S. Treasury Bond 30-Year Rate (Yield)</t>
+  </si>
+  <si>
+    <t>U.S. Treasury Inflation-Protected Security 30-Year Rate (Yield)</t>
+  </si>
+  <si>
+    <t>Estimated 30-Year Inflation Rate</t>
+  </si>
+  <si>
+    <t>as of 9/26/2022</t>
+  </si>
+  <si>
+    <t>Inflation-Adjusted Cost of Capital</t>
+  </si>
+  <si>
+    <t>Weighted average cost of capital minus expected inflation rate</t>
+  </si>
+  <si>
+    <t>Cost of Capital for Electricity Sector Projects</t>
+  </si>
+  <si>
+    <t>Projected Future Inflation Rate</t>
+  </si>
+  <si>
+    <t>Bloomberg</t>
+  </si>
+  <si>
+    <t>United States Rates &amp; Bonds</t>
+  </si>
+  <si>
+    <t>https://www.bloomberg.com/markets/rates-bonds/government-bonds/us</t>
+  </si>
+  <si>
+    <t>Compare 30-year treasury bond yield to 30-year treasury inflation-protected security (TIPS) yield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +210,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,7 +240,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -186,9 +252,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -505,11 +577,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F0629E-7DF7-4E6A-B1DA-78D3050B5FAD}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="87.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -520,63 +595,126 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>2021</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{867DFE11-7AC9-4394-8F96-3B3AEC2E1E67}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{867DFE11-7AC9-4394-8F96-3B3AEC2E1E67}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{2E89D36F-FC27-4D19-93B8-60E068C81CDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -584,55 +722,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0493C6E0-B904-42AD-8628-915D37F837B5}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="1" max="1" width="63" customWidth="1"/>
     <col min="2" max="3" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B4" s="4">
         <v>0.6</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C4" s="4">
         <v>0.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.08</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.08</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <f>SUMPRODUCT(B2:C2,B3:C3)</f>
+      <c r="B7" s="15">
+        <f>SUMPRODUCT(B4:C4,B5:C5)</f>
         <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="11">
+        <v>3.7400000000000003E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="14">
+        <f>B12-B13</f>
+        <v>2.1800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="13">
+        <f>B7-B15</f>
+        <v>7.4200000000000002E-2</v>
       </c>
     </row>
   </sheetData>
@@ -667,9 +864,9 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <f>'Lazard Data'!A6</f>
-        <v>9.6000000000000002E-2</v>
+      <c r="B2" s="12">
+        <f>Data!B20</f>
+        <v>7.4200000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>